<commit_message>
fixed bug for excel to xml tool
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Struct/NPC.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Struct/NPC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Struct\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Struct\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="79">
   <si>
     <t>Id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -264,6 +264,18 @@
   </si>
   <si>
     <t>BUFF免疫开关</t>
+  </si>
+  <si>
+    <t>SeedID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>种子ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -365,8 +377,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:I38" tableType="xml" totalsRowShown="0" connectionId="1">
-  <autoFilter ref="A1:I38"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:I39" tableType="xml" totalsRowShown="0" connectionId="1">
+  <autoFilter ref="A1:I39"/>
   <tableColumns count="9">
     <tableColumn id="1" uniqueName="Id" name="Id">
       <xmlColumnPr mapId="1" xpath="/Propertys/Property/@Id" xmlDataType="string"/>
@@ -663,9 +675,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -710,20 +724,20 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>46</v>
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
       </c>
       <c r="D2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -734,13 +748,13 @@
       <c r="H2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>50</v>
+      <c r="I2" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>46</v>
@@ -752,7 +766,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -764,12 +778,12 @@
         <v>49</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>46</v>
@@ -781,7 +795,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -793,12 +807,12 @@
         <v>49</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>46</v>
@@ -822,12 +836,12 @@
         <v>49</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>46</v>
@@ -851,24 +865,24 @@
         <v>49</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" t="b">
         <v>0</v>
       </c>
       <c r="D7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -879,14 +893,16 @@
       <c r="H7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="1"/>
+      <c r="I7" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" t="b">
         <v>0</v>
@@ -895,7 +911,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -910,7 +926,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>48</v>
@@ -937,7 +953,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>48</v>
@@ -964,7 +980,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>48</v>
@@ -976,7 +992,7 @@
         <v>0</v>
       </c>
       <c r="E11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -991,7 +1007,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>48</v>
@@ -1018,7 +1034,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>48</v>
@@ -1045,10 +1061,10 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
@@ -1072,7 +1088,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>46</v>
@@ -1081,7 +1097,7 @@
         <v>0</v>
       </c>
       <c r="D15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
@@ -1095,13 +1111,11 @@
       <c r="H15" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I15" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>46</v>
@@ -1125,12 +1139,12 @@
         <v>49</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>46</v>
@@ -1154,12 +1168,12 @@
         <v>49</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>46</v>
@@ -1183,12 +1197,12 @@
         <v>49</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>46</v>
@@ -1212,12 +1226,12 @@
         <v>49</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>46</v>
@@ -1241,12 +1255,12 @@
         <v>49</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>46</v>
@@ -1270,12 +1284,12 @@
         <v>49</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>46</v>
@@ -1299,12 +1313,12 @@
         <v>49</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>46</v>
@@ -1328,12 +1342,12 @@
         <v>49</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>46</v>
@@ -1357,12 +1371,12 @@
         <v>49</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>46</v>
@@ -1386,12 +1400,12 @@
         <v>49</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>46</v>
@@ -1415,12 +1429,12 @@
         <v>49</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>46</v>
@@ -1444,12 +1458,12 @@
         <v>49</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>46</v>
@@ -1473,12 +1487,12 @@
         <v>49</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>46</v>
@@ -1502,12 +1516,12 @@
         <v>49</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>46</v>
@@ -1531,12 +1545,12 @@
         <v>49</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>46</v>
@@ -1560,12 +1574,12 @@
         <v>49</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>46</v>
@@ -1589,18 +1603,18 @@
         <v>49</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D33" t="b">
         <v>1</v>
@@ -1618,12 +1632,12 @@
         <v>49</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>46</v>
@@ -1647,12 +1661,12 @@
         <v>49</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>46</v>
@@ -1676,12 +1690,12 @@
         <v>49</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>46</v>
@@ -1705,12 +1719,12 @@
         <v>49</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>46</v>
@@ -1734,43 +1748,73 @@
         <v>49</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D38" t="b">
+        <v>1</v>
+      </c>
+      <c r="E38" t="b">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A39" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C38" t="b">
-        <v>1</v>
-      </c>
-      <c r="D38" t="b">
-        <v>1</v>
-      </c>
-      <c r="E38" t="b">
-        <v>0</v>
-      </c>
-      <c r="F38">
-        <v>0</v>
-      </c>
-      <c r="G38">
-        <v>0</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I38" s="1" t="s">
+      <c r="B39" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" t="b">
+        <v>1</v>
+      </c>
+      <c r="D39" t="b">
+        <v>1</v>
+      </c>
+      <c r="E39" t="b">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I39" s="1" t="s">
         <v>75</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
set NPC HP property to public
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Struct/NPC.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Struct/NPC.xlsx
@@ -808,7 +808,7 @@
   <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -928,7 +928,7 @@
         <v>15</v>
       </c>
       <c r="C4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>

</xml_diff>